<commit_message>
Remove RestSharp and add more API methods (#2)
* Remove RestSharp
* More API methods
</commit_message>
<xml_diff>
--- a/ГенераторКода.xlsx
+++ b/ГенераторКода.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Дичь" sheetId="1" r:id="rId1"/>
     <sheet name="Operation" sheetId="2" r:id="rId2"/>
     <sheet name="Вид РПО" sheetId="3" r:id="rId3"/>
     <sheet name="Категория РПО" sheetId="4" r:id="rId4"/>
+    <sheet name="Телефон" sheetId="5" r:id="rId5"/>
+    <sheet name="качества адреса" sheetId="6" r:id="rId6"/>
+    <sheet name="нормализации адреса" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="472">
   <si>
     <t>Код операции</t>
   </si>
@@ -1205,6 +1208,234 @@
   </si>
   <si>
     <t>Комбинированное</t>
+  </si>
+  <si>
+    <t>CONFIRMED_MANUALLY</t>
+  </si>
+  <si>
+    <t>Подтверждено контролером</t>
+  </si>
+  <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>Корректный телефонный номер</t>
+  </si>
+  <si>
+    <t>GOOD_REPLACED_CODE</t>
+  </si>
+  <si>
+    <t>Изменен код телефонного номера</t>
+  </si>
+  <si>
+    <t>GOOD_REPLACED_NUMBER</t>
+  </si>
+  <si>
+    <t>Изменен номер телефона</t>
+  </si>
+  <si>
+    <t>GOOD_REPLACED_CODE_NUMBER</t>
+  </si>
+  <si>
+    <t>Изменен код и номер телефона</t>
+  </si>
+  <si>
+    <t>GOOD_CITY_CONFLICT</t>
+  </si>
+  <si>
+    <t>Конфликт по городу</t>
+  </si>
+  <si>
+    <t>GOOD_REGION_CONFLICT</t>
+  </si>
+  <si>
+    <t>Конфликт по региону</t>
+  </si>
+  <si>
+    <t>FOREIGN</t>
+  </si>
+  <si>
+    <t>Иностранный телефонный номер</t>
+  </si>
+  <si>
+    <t>CODE_AMBI</t>
+  </si>
+  <si>
+    <t>Неоднозначный код телефонного номера</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t>Пустой телефонный номер</t>
+  </si>
+  <si>
+    <t>GARBAGE</t>
+  </si>
+  <si>
+    <t>Телефонный номер содержит некорректные символы</t>
+  </si>
+  <si>
+    <t>GOOD_CITY</t>
+  </si>
+  <si>
+    <t>Восстановлен город в телефонном номере</t>
+  </si>
+  <si>
+    <t>GOOD_EXTRA_PHONE</t>
+  </si>
+  <si>
+    <t>Запись содержит более одного телефона</t>
+  </si>
+  <si>
+    <t>UNDEF</t>
+  </si>
+  <si>
+    <t>Телефон не может быть распознан</t>
+  </si>
+  <si>
+    <t>INCORRECT_DATA</t>
+  </si>
+  <si>
+    <t>Пригоден для почтовой рассылки</t>
+  </si>
+  <si>
+    <t>ON_DEMAND</t>
+  </si>
+  <si>
+    <t>POSTAL_BOX</t>
+  </si>
+  <si>
+    <t>Абонентский ящик</t>
+  </si>
+  <si>
+    <t>UNDEF_01</t>
+  </si>
+  <si>
+    <t>Не определен регион</t>
+  </si>
+  <si>
+    <t>UNDEF_02</t>
+  </si>
+  <si>
+    <t>Не определен город или населенный пункт</t>
+  </si>
+  <si>
+    <t>UNDEF_03</t>
+  </si>
+  <si>
+    <t>Не определена улица</t>
+  </si>
+  <si>
+    <t>UNDEF_04</t>
+  </si>
+  <si>
+    <t>Не определен номер дома</t>
+  </si>
+  <si>
+    <t>UNDEF_05</t>
+  </si>
+  <si>
+    <t>Не определена квартира/офис</t>
+  </si>
+  <si>
+    <t>UNDEF_06</t>
+  </si>
+  <si>
+    <t>Не определен</t>
+  </si>
+  <si>
+    <t>UNDEF_07</t>
+  </si>
+  <si>
+    <t>Иностранный адрес</t>
+  </si>
+  <si>
+    <t>VALIDATED</t>
+  </si>
+  <si>
+    <t>Уверенное распознавание</t>
+  </si>
+  <si>
+    <t>OVERRIDDEN</t>
+  </si>
+  <si>
+    <t>Распознан: адрес был перезаписан в справочнике</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_UNPARSED_PARTS</t>
+  </si>
+  <si>
+    <t>На проверку, неразобранные части</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_ASSUMPTION</t>
+  </si>
+  <si>
+    <t>На проверку, предположение</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_NO_MAIN_POINTS</t>
+  </si>
+  <si>
+    <t>На проверку, нет основных частей</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_NUMBER_STREET_ASSUMPTION</t>
+  </si>
+  <si>
+    <t>На проверку, предположение по улице</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_NO_KLADR_RECORD</t>
+  </si>
+  <si>
+    <t>На проверку, нет в КЛАДР</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HOUSE_WITHOUT_STREET_OR_NP</t>
+  </si>
+  <si>
+    <t>На проверку, нет улицы или населенного пункта</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HOUSE_EXTENSION_WITHOUT_HOUSE</t>
+  </si>
+  <si>
+    <t>На проверку, нет дома</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_HAS_AMBI</t>
+  </si>
+  <si>
+    <t>На проверку, неоднозначность</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_EXCEDED_HOUSE_NUMBER</t>
+  </si>
+  <si>
+    <t>На проверку, большой номер дома</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_INCORRECT_HOUSE</t>
+  </si>
+  <si>
+    <t>На проверку, некорректный дом</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_INCORRECT_HOUSE_EXTENSION</t>
+  </si>
+  <si>
+    <t>На проверку, некорректное расширение дома</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_FOREIGN</t>
+  </si>
+  <si>
+    <t>NOT_VALIDATED_DICTIONARY</t>
+  </si>
+  <si>
+    <t>На проверку, не по справочнику</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1478,16 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1273,7 +1513,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Код операции"/>
     <tableColumn id="2" name="Название операции"/>
-    <tableColumn id="3" name="Столбец1" dataDxfId="2">
+    <tableColumn id="3" name="Столбец1" dataDxfId="5">
       <calculatedColumnFormula>"/// &lt;summary&gt;
   /// "&amp;Таблица1[[#This Row],[Название операции]]&amp;"
   /// &lt;/summary&gt;
@@ -1290,7 +1530,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Значение"/>
     <tableColumn id="2" name="Описание"/>
-    <tableColumn id="3" name="Столбец1" dataDxfId="0">
+    <tableColumn id="3" name="Столбец1" dataDxfId="4">
       <calculatedColumnFormula>"/// &lt;summary&gt;
   /// "&amp;Таблица3[[#This Row],[Описание]]&amp;"
   /// &lt;/summary&gt;
@@ -1307,11 +1547,62 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Значение"/>
     <tableColumn id="2" name="Описание"/>
+    <tableColumn id="3" name="Столбец1" dataDxfId="3">
+      <calculatedColumnFormula>"/// &lt;summary&gt;
+  /// "&amp;Таблица4[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица4[[#This Row],[Значение]]&amp;","</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Значение"/>
+    <tableColumn id="2" name="Описание"/>
+    <tableColumn id="3" name="Столбец1" dataDxfId="2">
+      <calculatedColumnFormula>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица5" displayName="Таблица5" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Значение"/>
+    <tableColumn id="2" name="Описание"/>
     <tableColumn id="3" name="Столбец1" dataDxfId="1">
       <calculatedColumnFormula>"/// &lt;summary&gt;
-  /// "&amp;Таблица4[[#This Row],[Описание]]&amp;"
-  /// &lt;/summary&gt;
- "&amp;Таблица4[[#This Row],[Значение]]&amp;","</calculatedColumnFormula>
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Таблица6" displayName="Таблица6" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Значение"/>
+    <tableColumn id="2" name="Описание"/>
+    <tableColumn id="3" name="Столбец1" dataDxfId="0">
+      <calculatedColumnFormula>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7435,8 +7726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7866,7 +8157,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8074,4 +8365,844 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="159.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Подтверждено контролером
+  /// &lt;/summary&gt;
+ CONFIRMED_MANUALLY,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Корректный телефонный номер
+  /// &lt;/summary&gt;
+ GOOD,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Изменен код телефонного номера
+  /// &lt;/summary&gt;
+ GOOD_REPLACED_CODE,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Изменен номер телефона
+  /// &lt;/summary&gt;
+ GOOD_REPLACED_NUMBER,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B6" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Изменен код и номер телефона
+  /// &lt;/summary&gt;
+ GOOD_REPLACED_CODE_NUMBER,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Конфликт по городу
+  /// &lt;/summary&gt;
+ GOOD_CITY_CONFLICT,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" t="s">
+        <v>409</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Конфликт по региону
+  /// &lt;/summary&gt;
+ GOOD_REGION_CONFLICT,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Иностранный телефонный номер
+  /// &lt;/summary&gt;
+ FOREIGN,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Неоднозначный код телефонного номера
+  /// &lt;/summary&gt;
+ CODE_AMBI,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>414</v>
+      </c>
+      <c r="B11" t="s">
+        <v>415</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Пустой телефонный номер
+  /// &lt;/summary&gt;
+ EMPTY,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>416</v>
+      </c>
+      <c r="B12" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Телефонный номер содержит некорректные символы
+  /// &lt;/summary&gt;
+ GARBAGE,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>418</v>
+      </c>
+      <c r="B13" t="s">
+        <v>419</v>
+      </c>
+      <c r="C13" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Восстановлен город в телефонном номере
+  /// &lt;/summary&gt;
+ GOOD_CITY,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B14" t="s">
+        <v>421</v>
+      </c>
+      <c r="C14" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Запись содержит более одного телефона
+  /// &lt;/summary&gt;
+ GOOD_EXTRA_PHONE,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B15" t="s">
+        <v>423</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Телефон не может быть распознан
+  /// &lt;/summary&gt;
+ UNDEF,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>424</v>
+      </c>
+      <c r="B16" t="s">
+        <v>423</v>
+      </c>
+      <c r="C16" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица2[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица2[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Телефон не может быть распознан
+  /// &lt;/summary&gt;
+ INCORRECT_DATA,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Пригоден для почтовой рассылки
+  /// &lt;/summary&gt;
+ GOOD,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// До востребования
+  /// &lt;/summary&gt;
+ ON_DEMAND,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Абонентский ящик
+  /// &lt;/summary&gt;
+ POSTAL_BOX,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определен регион
+  /// &lt;/summary&gt;
+ UNDEF_01,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>431</v>
+      </c>
+      <c r="B6" t="s">
+        <v>432</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определен город или населенный пункт
+  /// &lt;/summary&gt;
+ UNDEF_02,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определена улица
+  /// &lt;/summary&gt;
+ UNDEF_03,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определен номер дома
+  /// &lt;/summary&gt;
+ UNDEF_04,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B9" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определена квартира/офис
+  /// &lt;/summary&gt;
+ UNDEF_05,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>439</v>
+      </c>
+      <c r="B10" t="s">
+        <v>440</v>
+      </c>
+      <c r="C10" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Не определен
+  /// &lt;/summary&gt;
+ UNDEF_06,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B11" t="s">
+        <v>442</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица5[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица5[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Иностранный адрес
+  /// &lt;/summary&gt;
+ UNDEF_07,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="127.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Подтверждено контролером
+  /// &lt;/summary&gt;
+ CONFIRMED_MANUALLY,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Уверенное распознавание
+  /// &lt;/summary&gt;
+ VALIDATED,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Распознан: адрес был перезаписан в справочнике
+  /// &lt;/summary&gt;
+ OVERRIDDEN,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, неразобранные части
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_UNPARSED_PARTS,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B6" t="s">
+        <v>450</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, предположение
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_ASSUMPTION,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, нет основных частей
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_NO_MAIN_POINTS,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, предположение по улице
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_NUMBER_STREET_ASSUMPTION,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>455</v>
+      </c>
+      <c r="B9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, нет в КЛАДР
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_NO_KLADR_RECORD,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B10" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, нет улицы или населенного пункта
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HOUSE_WITHOUT_STREET_OR_NP,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, нет дома
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HOUSE_EXTENSION_WITHOUT_HOUSE,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B12" t="s">
+        <v>462</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, неоднозначность
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_HAS_AMBI,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>463</v>
+      </c>
+      <c r="B13" t="s">
+        <v>464</v>
+      </c>
+      <c r="C13" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, большой номер дома
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_EXCEDED_HOUSE_NUMBER,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>465</v>
+      </c>
+      <c r="B14" t="s">
+        <v>466</v>
+      </c>
+      <c r="C14" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, некорректный дом
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_INCORRECT_HOUSE,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>467</v>
+      </c>
+      <c r="B15" t="s">
+        <v>468</v>
+      </c>
+      <c r="C15" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, некорректное расширение дома
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_INCORRECT_HOUSE_EXTENSION,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>469</v>
+      </c>
+      <c r="B16" t="s">
+        <v>442</v>
+      </c>
+      <c r="C16" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// Иностранный адрес
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_FOREIGN,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>470</v>
+      </c>
+      <c r="B17" t="s">
+        <v>471</v>
+      </c>
+      <c r="C17" t="str">
+        <f>"/// &lt;summary&gt;
+  /// "&amp;Таблица6[[#This Row],[Описание]]&amp;"
+  /// &lt;/summary&gt;
+ "&amp;Таблица6[[#This Row],[Значение]]&amp;","</f>
+        <v>/// &lt;summary&gt;
+  /// На проверку, не по справочнику
+  /// &lt;/summary&gt;
+ NOT_VALIDATED_DICTIONARY,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>